<commit_message>
Added Alpabetical page controller and view. Added connection to DB via Dapper. Added Bird, Image and Family DTOs. Added tab control to manage the alphabetical display. Implemented partial view to show card blurbs upon selecting letter
</commit_message>
<xml_diff>
--- a/Extras/AvesTables.xlsx
+++ b/Extras/AvesTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bird" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="1019">
   <si>
     <t>Id</t>
   </si>
@@ -3040,6 +3040,39 @@
   </si>
   <si>
     <t>Hudsonian whimbrel</t>
+  </si>
+  <si>
+    <t>BirdId</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Coordinate</t>
+  </si>
+  <si>
+    <t>KeyImage</t>
+  </si>
+  <si>
+    <t>dsc5740w</t>
+  </si>
+  <si>
+    <t>dsc09835w</t>
+  </si>
+  <si>
+    <t>rcc05368w</t>
+  </si>
+  <si>
+    <t>rcc09277_1w</t>
   </si>
 </sst>
 </file>
@@ -3398,8 +3431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="B387" sqref="B387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9143,14 +9176,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A22:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>143</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>388</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>